<commit_message>
files sended to manufacturing
</commit_message>
<xml_diff>
--- a/Producto Final/COMECA - MCU Board/Project Outputs for COMECA - MCU Board/PickPlace - JLC.xlsx
+++ b/Producto Final/COMECA - MCU Board/Project Outputs for COMECA - MCU Board/PickPlace - JLC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcelo\Documents\GitHub\DisenioBJAM\Producto Final\COMECA - MCU Board\Project Outputs for COMECA - MCU Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5E0842-2C49-43AA-A95F-3586D50CB008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6946D1E8-472C-49FC-82F4-7CE8636C58D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="157">
   <si>
     <t>Designator</t>
   </si>
@@ -69,21 +69,12 @@
     <t>0603-IND-MURATA</t>
   </si>
   <si>
-    <t>11.3030mm</t>
-  </si>
-  <si>
-    <t>46.1010mm</t>
-  </si>
-  <si>
     <t>180</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>12.0280mm</t>
-  </si>
-  <si>
     <t>CE4</t>
   </si>
   <si>
@@ -499,6 +490,12 @@
   </si>
   <si>
     <t>28.8072mm</t>
+  </si>
+  <si>
+    <t>45.7200mm</t>
+  </si>
+  <si>
+    <t>11.6470mm</t>
   </si>
 </sst>
 </file>
@@ -867,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -910,1157 +907,1157 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>22</v>
+        <v>155</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>22</v>
+        <v>155</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>21</v>
+        <v>156</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>21</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="G4" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="G5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="G12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="K12" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K13" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>70</v>
-      </c>
       <c r="I14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J14" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="J14" s="5" t="s">
-        <v>70</v>
-      </c>
       <c r="K14" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="J16" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="5" t="s">
+      <c r="K16" s="6" t="s">
         <v>74</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="K17" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="5" t="s">
+      <c r="K18" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="K19" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J20" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>96</v>
-      </c>
       <c r="K20" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="5" t="s">
+      <c r="F21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="J21" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="K21" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K22" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J24" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="K24" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J25" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D25" s="5" t="s">
+      <c r="K25" s="6" t="s">
         <v>116</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="K25" s="6" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="K26" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="K28" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D29" s="5" t="s">
+      <c r="K29" s="6" t="s">
         <v>133</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J30" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="K30" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="K30" s="3" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J32" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="K32" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="J33" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D33" s="5" t="s">
+      <c r="K33" s="6" t="s">
         <v>149</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="J33" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="J34" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D34" s="2" t="s">
+      <c r="K34" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="K34" s="3" t="s">
-        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>